<commit_message>
Some files Left Behind
</commit_message>
<xml_diff>
--- a/lib/seeds/FinanceMaster.xlsx
+++ b/lib/seeds/FinanceMaster.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21015" windowHeight="8205" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="132" windowWidth="21012" windowHeight="8148" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AircraftLeasing" sheetId="1" r:id="rId1"/>
     <sheet name="Bank" sheetId="2" r:id="rId2"/>
     <sheet name="CreditBook" sheetId="4" r:id="rId3"/>
+    <sheet name="LeaseBook" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>name</t>
   </si>
@@ -178,13 +179,19 @@
   </si>
   <si>
     <t>turn</t>
+  </si>
+  <si>
+    <t>leaser_id</t>
+  </si>
+  <si>
+    <t>plane_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,9 +237,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Ofis Teması">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Ofis">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -270,7 +277,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Ofis">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -304,6 +311,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -338,9 +346,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Ofis">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -513,24 +522,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -547,7 +556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -564,7 +573,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -581,7 +590,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -598,7 +607,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -615,7 +624,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -632,7 +641,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -649,7 +658,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -666,7 +675,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -683,7 +692,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -700,7 +709,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -717,7 +726,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -740,22 +749,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -778,7 +790,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -801,7 +813,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -824,7 +836,7 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -847,7 +859,7 @@
         <v>900000</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -870,7 +882,7 @@
         <v>8400000</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -893,7 +905,7 @@
         <v>9600000</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -916,7 +928,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -939,7 +951,7 @@
         <v>60000000</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -962,7 +974,7 @@
         <v>80000000</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -991,21 +1003,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1026,6 +1038,32 @@
       </c>
       <c r="G1" t="s">
         <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>